<commit_message>
Finished converting file I/O actions and thunk actions
</commit_message>
<xml_diff>
--- a/src/data/TDE5.xlsx
+++ b/src/data/TDE5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6290" uniqueCount="4379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6303" uniqueCount="4379">
   <si>
     <t>id</t>
   </si>
@@ -65406,10 +65406,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -65434,10 +65434,11 @@
     <col min="19" max="20" width="10.6640625" style="1" customWidth="1"/>
     <col min="21" max="21" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.6640625" style="1"/>
+    <col min="23" max="23" width="13.265625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -65504,8 +65505,11 @@
       <c r="V1" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W1" s="5" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -65550,8 +65554,11 @@
       <c r="V2" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W2" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -65602,8 +65609,11 @@
       <c r="V3" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W3" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -65648,8 +65658,11 @@
       <c r="V4" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W4" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -65700,8 +65713,11 @@
       <c r="V5" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W5" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -65752,8 +65768,11 @@
       <c r="V6" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W6" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -65804,8 +65823,11 @@
       <c r="V7" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W7" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -65856,8 +65878,11 @@
       <c r="V8" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W8" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -65924,8 +65949,11 @@
       <c r="V9" s="3" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W9" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -65992,8 +66020,11 @@
       <c r="V10" s="3" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W10" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -66060,8 +66091,11 @@
       <c r="V11" s="3" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W11" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -66118,8 +66152,11 @@
       <c r="V12" s="3" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="W12" s="22" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -66183,6 +66220,9 @@
       </c>
       <c r="V13" s="3" t="s">
         <v>301</v>
+      </c>
+      <c r="W13" s="22" t="s">
+        <v>2529</v>
       </c>
     </row>
   </sheetData>
@@ -66198,8 +66238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L2:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -67397,8 +67437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Refactored some Flux implementation links and redesigned a few more Dialogs, added SpellInfo
</commit_message>
<xml_diff>
--- a/src/data/TDE5.xlsx
+++ b/src/data/TDE5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6587" uniqueCount="4650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6821" uniqueCount="4651">
   <si>
     <t>id</t>
   </si>
@@ -13998,6 +13998,9 @@
   </si>
   <si>
     <t>3?4&amp;9?4&amp;13?2</t>
+  </si>
+  <si>
+    <t>US25101&amp;US25004</t>
   </si>
 </sst>
 </file>
@@ -14180,7 +14183,10 @@
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="215">
+  <dxfs count="216">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -15382,7 +15388,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="214"/>
+      <tableStyleElement type="headerRow" dxfId="215"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -16759,7 +16765,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="213" dataDxfId="212">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="214" dataDxfId="213">
   <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000011000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16768,15 +16774,15 @@
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="211"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="210"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="212"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="211"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:F60" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:F60" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
   <autoFilter ref="A1:F60" xr:uid="{00000000-0009-0000-0100-000007000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16789,20 +16795,20 @@
     <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="check" dataDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="skt" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="be" dataDxfId="115"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="gr" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="check" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="skt" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="be" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="gr" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:J234" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
-  <autoFilter ref="A1:J234" xr:uid="{00000000-0009-0000-0100-000004000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:K234" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
+  <autoFilter ref="A1:K234" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -16813,25 +16819,27 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
     <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="check" dataDxfId="109"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="mod" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="skt" dataDxfId="107"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="trad" dataDxfId="106"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="subtrad" dataDxfId="105"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="merk" dataDxfId="104"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="gr" dataDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="req" dataDxfId="102"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="check" dataDxfId="110"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="mod" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="skt" dataDxfId="108"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="trad" dataDxfId="107"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="subtrad" dataDxfId="106"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="merk" dataDxfId="105"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="gr" dataDxfId="104"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="req" dataDxfId="103"/>
+    <tableColumn id="11" xr3:uid="{6093D09C-4084-4E7B-85B0-373570094BC3}" name="src" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table14" displayName="Table14" ref="A1:E44" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table14" displayName="Table14" ref="A1:E44" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <autoFilter ref="A1:E44" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16840,18 +16848,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="trad" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="merk" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="req" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="trad" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="merk" dataDxfId="97"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="req" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:H193" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:H193" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:H193" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16863,21 +16871,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="check" dataDxfId="90"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="mod" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="skt" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="trad" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="aspc" dataDxfId="86"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="gr" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="check" dataDxfId="91"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="mod" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="skt" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="trad" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="aspc" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="gr" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table1417" displayName="Table1417" ref="A1:E13" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table1417" displayName="Table1417" ref="A1:E13" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
   <autoFilter ref="A1:E13" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16886,18 +16894,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="trad" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="aspc" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="req" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="trad" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="aspc" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="req" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:H781" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:H781" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:H781" xr:uid="{00000000-0009-0000-0100-000006000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16909,21 +16917,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="ap" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="tiers" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="max" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="sel" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="req" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="gr" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="ap" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="tiers" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="max" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="sel" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="req" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="gr" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table10" displayName="Table10" ref="A1:E111" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table10" displayName="Table10" ref="A1:E111" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A1:E111" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16932,51 +16940,51 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="req" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="cost" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="sec" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="req" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="cost" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="sec" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:D76" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="cont" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="ext" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="cont" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="ext" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle19212324" displayName="Tabelle19212324" ref="A1:C19" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle19212324" displayName="Tabelle19212324" ref="A1:C19" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A1:C19" xr:uid="{00000000-0009-0000-0100-000017000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="talent" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="talent" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table11" displayName="Table11" ref="A1:F36" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table11" displayName="Table11" ref="A1:F36" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:F36" xr:uid="{00000000-0009-0000-0100-00000B000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -16986,19 +16994,19 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="id" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="name" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="languages" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="cost" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="cont" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="ext" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="id" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="name" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="languages" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="cost" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="cont" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="ext" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I8" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I8" totalsRowShown="0" headerRowDxfId="210" dataDxfId="209">
   <autoFilter ref="A1:I8" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17011,22 +17019,22 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="207"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="206"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="ap" dataDxfId="205"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="maxAttributeValue" dataDxfId="204"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="maxSkillRating" dataDxfId="203"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="maxCombatTechniqueRating" dataDxfId="202"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="maxTotalAttributeValues" dataDxfId="201"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="maxSpellsLiturgies" dataDxfId="200"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="maxUnfamiliarSpells" dataDxfId="199"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="208"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="207"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="ap" dataDxfId="206"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="maxAttributeValue" dataDxfId="205"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="maxSkillRating" dataDxfId="204"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="maxCombatTechniqueRating" dataDxfId="203"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="maxTotalAttributeValues" dataDxfId="202"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="maxSpellsLiturgies" dataDxfId="201"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="maxUnfamiliarSpells" dataDxfId="200"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Tabelle192123" displayName="Tabelle192123" ref="A1:E7" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Tabelle192123" displayName="Tabelle192123" ref="A1:E7" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A1:E7" xr:uid="{00000000-0009-0000-0100-000016000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17035,18 +17043,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="id" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="name" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="cost" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="gr" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="tier" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="id" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="name" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="cost" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="gr" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="tier" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table15" displayName="Table15" ref="A1:F466" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" dataCellStyle="Excel Built-in Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table15" displayName="Table15" ref="A1:F466" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" dataCellStyle="Excel Built-in Normal">
   <autoFilter ref="A1:F466" xr:uid="{00000000-0009-0000-0100-00000F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17056,56 +17064,56 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="name" dataDxfId="31" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="target" dataDxfId="30" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="tier" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="req" dataDxfId="28" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="cost" dataDxfId="27" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="id" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="name" dataDxfId="32" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="target" dataDxfId="31" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="tier" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="req" dataDxfId="29" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="cost" dataDxfId="28" dataCellStyle="Excel Built-in Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:Y484" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:Y484" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:Y484" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <sortState ref="A2:Y484">
     <sortCondition ref="A1:A484"/>
   </sortState>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="id" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="name" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="price" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="weight" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="gr" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1500-000006000000}" name="ct" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1500-000007000000}" name="ddn" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1500-000014000000}" name="dds" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1500-000008000000}" name="df" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1500-000009000000}" name="db" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1500-00000A000000}" name="at" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1500-00000B000000}" name="pa" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1500-00000C000000}" name="re" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1500-00000D000000}" name="length" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1500-00000E000000}" name="stp" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1500-000015000000}" name="range" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1500-00000F000000}" name="rt" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1500-000010000000}" name="am" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1500-000011000000}" name="pro" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1500-000012000000}" name="enc" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1500-000013000000}" name="addp" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-1500-000019000000}" name="armty" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-1500-000016000000}" name="pryw" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-1500-000017000000}" name="two" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1500-000018000000}" name="imp" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="id" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="name" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="price" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="weight" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="gr" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1500-000006000000}" name="ct" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1500-000007000000}" name="ddn" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1500-000014000000}" name="dds" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1500-000008000000}" name="df" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1500-000009000000}" name="db" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1500-00000A000000}" name="at" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1500-00000B000000}" name="pa" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1500-00000C000000}" name="re" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1500-00000D000000}" name="length" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1500-00000E000000}" name="stp" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1500-000015000000}" name="range" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1500-00000F000000}" name="rt" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1500-000010000000}" name="am" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1500-000011000000}" name="pro" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1500-000012000000}" name="enc" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1500-000013000000}" name="addp" dataDxfId="5"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-1500-000019000000}" name="armty" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-1500-000016000000}" name="pryw" dataDxfId="3"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-1500-000017000000}" name="two" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1500-000018000000}" name="imp" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:N1048576" totalsRowShown="0" headerRowDxfId="198" dataDxfId="197">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:N1048576" totalsRowShown="0" headerRowDxfId="199" dataDxfId="198">
   <autoFilter ref="A1:N1048576" xr:uid="{00000000-0009-0000-0100-000012000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17123,27 +17131,27 @@
     <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="196"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="195"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ap" dataDxfId="194"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="lang" dataDxfId="193"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="literacy" dataDxfId="192"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="social" dataDxfId="191"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="typ_prof" dataDxfId="190"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="typ_adv" dataDxfId="189"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="typ_dadv" dataDxfId="188"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="untyp_adv" dataDxfId="187"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="untyp_dadv" dataDxfId="186"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="typ_talents" dataDxfId="185"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="untyp_talents" dataDxfId="184"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="talents" dataDxfId="183"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="197"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="196"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ap" dataDxfId="195"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="lang" dataDxfId="194"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="literacy" dataDxfId="193"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="social" dataDxfId="192"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="typ_prof" dataDxfId="191"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="typ_adv" dataDxfId="190"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="typ_dadv" dataDxfId="189"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="untyp_adv" dataDxfId="188"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="untyp_dadv" dataDxfId="187"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="typ_talents" dataDxfId="186"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="untyp_talents" dataDxfId="185"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="talents" dataDxfId="184"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:T95" totalsRowShown="0" headerRowDxfId="182" dataDxfId="181">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:T95" totalsRowShown="0" headerRowDxfId="183" dataDxfId="182">
   <autoFilter ref="A1:T95" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17167,33 +17175,33 @@
     <filterColumn colId="19" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="180"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="179"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ap" dataDxfId="178"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="pre_req" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="req" dataDxfId="176"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="sel" dataDxfId="175"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="sa" dataDxfId="174"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="combattech" dataDxfId="173"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="talents" dataDxfId="172"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="spells" dataDxfId="171"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="chants" dataDxfId="170"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="181"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="180"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ap" dataDxfId="179"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="pre_req" dataDxfId="178"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="req" dataDxfId="177"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="sel" dataDxfId="176"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="sa" dataDxfId="175"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="combattech" dataDxfId="174"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="talents" dataDxfId="173"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="spells" dataDxfId="172"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="chants" dataDxfId="171"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0300-000017000000}" name="blessings"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="typ_adv" dataDxfId="169"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="typ_dadv" dataDxfId="168"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="untyp_adv" dataDxfId="167"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="untyp_dadv" dataDxfId="166"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="vars" dataDxfId="165"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="gr" dataDxfId="164"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0300-000018000000}" name="sgr" dataDxfId="163"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="src" dataDxfId="162"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="typ_adv" dataDxfId="170"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="typ_dadv" dataDxfId="169"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="untyp_adv" dataDxfId="168"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="untyp_dadv" dataDxfId="167"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="vars" dataDxfId="166"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="gr" dataDxfId="165"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0300-000018000000}" name="sgr" dataDxfId="164"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="src" dataDxfId="163"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:J1048576" totalsRowShown="0" headerRowDxfId="161" dataDxfId="160">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:J1048576" totalsRowShown="0" headerRowDxfId="162" dataDxfId="161">
   <autoFilter ref="A1:J1048576" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17207,23 +17215,23 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="159"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="158"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ap" dataDxfId="157"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="pre_req" dataDxfId="156"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="req" dataDxfId="155"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="sel" dataDxfId="154"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="sa" dataDxfId="153"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="combattech" dataDxfId="152"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="talents" dataDxfId="151"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="spells" dataDxfId="150"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="160"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="159"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ap" dataDxfId="158"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="pre_req" dataDxfId="157"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="req" dataDxfId="156"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="sel" dataDxfId="155"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="sa" dataDxfId="154"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="combattech" dataDxfId="153"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="talents" dataDxfId="152"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="spells" dataDxfId="151"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:G76" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:G76" totalsRowShown="0" headerRowDxfId="150" dataDxfId="149">
   <autoFilter ref="A1:G76" xr:uid="{00000000-0009-0000-0100-000008000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17234,20 +17242,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="147"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="146"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="ap" dataDxfId="145"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="tiers" dataDxfId="144"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="max" dataDxfId="143"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="142"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="req" dataDxfId="141"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="ap" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="tiers" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="max" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="143"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="req" dataDxfId="142"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G72" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G72" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140">
   <autoFilter ref="A1:G72" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17258,45 +17266,45 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="138"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="137"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="ap" dataDxfId="136"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="tiers" dataDxfId="135"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="max" dataDxfId="134"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="133"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="req" dataDxfId="132"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="138"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="ap" dataDxfId="137"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="tiers" dataDxfId="136"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="max" dataDxfId="135"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="req" dataDxfId="133"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle19" displayName="Tabelle19" ref="A1:C15" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle19" displayName="Tabelle19" ref="A1:C15" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131">
   <autoFilter ref="A1:C15" xr:uid="{00000000-0009-0000-0100-000013000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tier" dataDxfId="127"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="130"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="129"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tier" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle1921" displayName="Tabelle1921" ref="A1:C10" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle1921" displayName="Tabelle1921" ref="A1:C10" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
   <autoFilter ref="A1:C10" xr:uid="{00000000-0009-0000-0100-000014000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="124"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="123"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="tier" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="tier" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17601,8 +17609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19678,10 +19686,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:J234"/>
+  <dimension ref="A1:K234"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19695,10 +19703,11 @@
     <col min="7" max="7" width="8.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.796875" style="1" customWidth="1"/>
     <col min="9" max="10" width="4.19921875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.6640625" style="1"/>
+    <col min="11" max="11" width="7.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -19729,8 +19738,11 @@
       <c r="J1" s="5" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" s="5" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -19752,8 +19764,11 @@
       <c r="I2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K2" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -19775,8 +19790,11 @@
       <c r="I3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -19798,8 +19816,11 @@
       <c r="I4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K4" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -19821,8 +19842,11 @@
       <c r="I5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K5" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -19844,8 +19868,11 @@
       <c r="I6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K6" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -19870,8 +19897,11 @@
       <c r="I7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K7" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -19896,8 +19926,11 @@
       <c r="I8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K8" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -19922,8 +19955,11 @@
       <c r="I9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K9" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -19948,8 +19984,11 @@
       <c r="I10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K10" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -19971,8 +20010,11 @@
       <c r="I11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K11" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -19994,8 +20036,11 @@
       <c r="I12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K12" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -20017,8 +20062,11 @@
       <c r="I13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K13" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -20040,8 +20088,11 @@
       <c r="I14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K14" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -20066,8 +20117,11 @@
       <c r="I15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K15" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -20089,8 +20143,11 @@
       <c r="I16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K16" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -20115,8 +20172,11 @@
       <c r="I17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K17" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -20138,8 +20198,11 @@
       <c r="I18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K18" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -20161,8 +20224,11 @@
       <c r="I19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K19" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -20184,8 +20250,11 @@
       <c r="I20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K20" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -20210,8 +20279,11 @@
       <c r="I21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K21" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -20233,8 +20305,11 @@
       <c r="I22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K22" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -20256,8 +20331,11 @@
       <c r="I23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K23" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -20279,8 +20357,11 @@
       <c r="I24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K24" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -20302,8 +20383,11 @@
       <c r="I25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K25" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -20325,8 +20409,11 @@
       <c r="I26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K26" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -20348,8 +20435,11 @@
       <c r="I27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K27" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -20371,8 +20461,11 @@
       <c r="I28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K28" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -20394,8 +20487,11 @@
       <c r="I29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K29" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -20417,8 +20513,11 @@
       <c r="I30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K30" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -20440,8 +20539,11 @@
       <c r="I31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K31" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -20466,8 +20568,11 @@
       <c r="I32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K32" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -20489,8 +20594,11 @@
       <c r="I33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K33" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -20512,8 +20620,11 @@
       <c r="I34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K34" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -20535,8 +20646,11 @@
       <c r="I35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K35" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -20561,8 +20675,11 @@
       <c r="I36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K36" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -20587,8 +20704,11 @@
       <c r="I37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K37" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -20613,8 +20733,11 @@
       <c r="I38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K38" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -20636,8 +20759,11 @@
       <c r="I39" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K39" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -20659,8 +20785,11 @@
       <c r="I40" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K40" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -20685,8 +20814,11 @@
       <c r="I41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K41" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -20708,8 +20840,11 @@
       <c r="I42" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K42" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -20731,8 +20866,11 @@
       <c r="I43" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K43" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -20754,8 +20892,11 @@
       <c r="I44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K44" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -20777,8 +20918,11 @@
       <c r="I45" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K45" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -20800,8 +20944,11 @@
       <c r="I46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K46" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -20823,8 +20970,11 @@
       <c r="I47" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K47" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -20849,8 +20999,11 @@
       <c r="J48" s="1" t="s">
         <v>3487</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K48" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -20875,8 +21028,11 @@
       <c r="J49" s="1" t="s">
         <v>3485</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K49" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -20901,8 +21057,11 @@
       <c r="J50" s="1" t="s">
         <v>3488</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K50" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -20927,8 +21086,11 @@
       <c r="J51" s="1" t="s">
         <v>3486</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K51" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -20950,8 +21112,11 @@
       <c r="I52" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K52" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -20976,8 +21141,11 @@
       <c r="I53" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K53" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -21002,8 +21170,11 @@
       <c r="I54" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K54" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -21025,8 +21196,11 @@
       <c r="I55" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K55" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -21051,8 +21225,11 @@
       <c r="I56" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K56" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -21077,8 +21254,11 @@
       <c r="I57" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K57" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -21103,8 +21283,11 @@
       <c r="I58" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K58" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -21129,8 +21312,11 @@
       <c r="I59" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K59" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -21155,8 +21341,11 @@
       <c r="I60" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K60" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -21181,8 +21370,11 @@
       <c r="I61" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K61" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -21207,8 +21399,11 @@
       <c r="I62" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K62" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -21230,8 +21425,11 @@
       <c r="I63" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K63" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -21253,8 +21451,11 @@
       <c r="I64" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K64" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -21276,8 +21477,11 @@
       <c r="I65" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K65" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -21299,8 +21503,11 @@
       <c r="I66" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K66" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -21322,8 +21529,11 @@
       <c r="I67" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K67" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -21345,8 +21555,11 @@
       <c r="I68" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K68" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -21368,8 +21581,11 @@
       <c r="I69" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K69" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -21391,8 +21607,11 @@
       <c r="I70" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K70" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -21414,8 +21633,11 @@
       <c r="I71" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K71" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -21437,8 +21659,11 @@
       <c r="I72" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K72" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -21460,8 +21685,11 @@
       <c r="I73" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K73" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -21483,8 +21711,11 @@
       <c r="I74" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K74" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -21506,8 +21737,11 @@
       <c r="I75" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K75" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -21529,8 +21763,11 @@
       <c r="I76" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K76" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -21552,8 +21789,11 @@
       <c r="I77" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K77" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -21575,8 +21815,11 @@
       <c r="I78" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K78" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -21598,8 +21841,11 @@
       <c r="I79" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K79" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -21621,8 +21867,11 @@
       <c r="I80" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K80" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -21644,8 +21893,11 @@
       <c r="I81" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K81" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -21667,8 +21919,11 @@
       <c r="I82" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K82" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -21690,8 +21945,11 @@
       <c r="I83" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K83" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -21713,8 +21971,11 @@
       <c r="I84" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K84" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -21736,8 +21997,11 @@
       <c r="I85" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K85" s="1" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -21759,8 +22023,11 @@
       <c r="I86" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K86" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -21782,8 +22049,11 @@
       <c r="I87" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K87" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -21805,8 +22075,11 @@
       <c r="I88" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K88" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -21828,8 +22101,11 @@
       <c r="I89" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K89" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -21851,8 +22127,11 @@
       <c r="I90" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K90" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -21874,8 +22153,11 @@
       <c r="I91" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K91" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -21897,8 +22179,11 @@
       <c r="I92" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K92" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -21920,8 +22205,11 @@
       <c r="I93" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K93" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -21943,8 +22231,11 @@
       <c r="I94" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K94" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -21966,8 +22257,11 @@
       <c r="I95" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K95" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -21989,8 +22283,11 @@
       <c r="I96" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K96" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -22012,8 +22309,11 @@
       <c r="I97" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K97" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -22035,8 +22335,11 @@
       <c r="I98" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K98" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -22058,8 +22361,11 @@
       <c r="I99" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K99" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -22081,8 +22387,11 @@
       <c r="I100" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K100" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -22104,8 +22413,11 @@
       <c r="I101" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K101" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -22127,8 +22439,11 @@
       <c r="I102" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K102" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -22150,8 +22465,11 @@
       <c r="I103" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K103" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -22173,8 +22491,11 @@
       <c r="I104" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K104" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -22196,8 +22517,11 @@
       <c r="I105" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K105" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -22219,8 +22543,11 @@
       <c r="I106" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K106" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -22242,8 +22569,11 @@
       <c r="I107" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K107" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -22265,8 +22595,11 @@
       <c r="I108" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K108" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -22288,8 +22621,11 @@
       <c r="I109" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K109" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -22311,8 +22647,11 @@
       <c r="I110" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K110" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -22334,8 +22673,11 @@
       <c r="I111" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K111" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -22357,8 +22699,11 @@
       <c r="I112" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K112" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -22380,8 +22725,11 @@
       <c r="I113" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K113" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -22403,8 +22751,11 @@
       <c r="I114" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K114" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -22426,8 +22777,11 @@
       <c r="I115" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K115" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -22449,8 +22803,11 @@
       <c r="I116" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K116" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -22472,8 +22829,11 @@
       <c r="I117" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K117" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -22495,8 +22855,11 @@
       <c r="I118" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K118" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -22518,8 +22881,11 @@
       <c r="I119" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K119" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -22541,8 +22907,11 @@
       <c r="I120" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K120" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -22564,8 +22933,11 @@
       <c r="I121" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K121" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -22587,8 +22959,11 @@
       <c r="I122" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K122" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -22610,8 +22985,11 @@
       <c r="I123" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K123" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -22633,8 +23011,11 @@
       <c r="I124" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K124" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -22656,8 +23037,11 @@
       <c r="I125" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K125" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -22679,8 +23063,11 @@
       <c r="I126" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K126" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -22702,8 +23089,11 @@
       <c r="I127" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K127" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -22725,8 +23115,11 @@
       <c r="I128" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K128" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -22748,8 +23141,11 @@
       <c r="I129" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K129" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -22771,8 +23167,11 @@
       <c r="I130" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K130" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -22794,8 +23193,11 @@
       <c r="I131" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K131" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -22817,8 +23219,11 @@
       <c r="I132" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K132" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -22840,8 +23245,11 @@
       <c r="I133" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K133" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -22863,8 +23271,11 @@
       <c r="I134" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K134" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -22886,8 +23297,11 @@
       <c r="I135" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K135" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -22909,8 +23323,11 @@
       <c r="I136" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K136" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -22932,8 +23349,11 @@
       <c r="I137" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K137" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -22955,8 +23375,11 @@
       <c r="I138" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K138" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -22978,8 +23401,11 @@
       <c r="I139" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K139" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -23001,8 +23427,11 @@
       <c r="I140" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K140" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -23024,8 +23453,11 @@
       <c r="I141" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K141" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -23047,8 +23479,11 @@
       <c r="I142" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K142" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -23070,8 +23505,11 @@
       <c r="I143" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K143" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -23093,8 +23531,11 @@
       <c r="I144" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K144" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -23116,8 +23557,11 @@
       <c r="I145" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K145" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -23139,8 +23583,11 @@
       <c r="I146" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K146" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -23162,8 +23609,11 @@
       <c r="I147" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K147" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -23185,8 +23635,11 @@
       <c r="I148" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K148" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -23208,8 +23661,11 @@
       <c r="I149" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K149" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -23231,8 +23687,11 @@
       <c r="I150" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K150" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -23254,8 +23713,11 @@
       <c r="I151" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K151" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -23277,8 +23739,11 @@
       <c r="I152" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K152" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -23300,8 +23765,11 @@
       <c r="I153" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K153" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -23323,8 +23791,11 @@
       <c r="I154" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K154" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -23346,8 +23817,11 @@
       <c r="I155" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K155" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -23369,8 +23843,11 @@
       <c r="I156" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K156" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -23392,8 +23869,11 @@
       <c r="I157" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K157" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -23415,8 +23895,11 @@
       <c r="I158" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K158" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -23438,8 +23921,11 @@
       <c r="I159" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K159" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -23461,8 +23947,11 @@
       <c r="I160" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K160" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -23484,8 +23973,11 @@
       <c r="I161" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K161" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -23507,8 +23999,11 @@
       <c r="I162" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K162" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -23530,8 +24025,11 @@
       <c r="I163" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K163" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -23553,8 +24051,11 @@
       <c r="I164" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K164" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -23576,8 +24077,11 @@
       <c r="I165" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K165" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -23599,8 +24103,11 @@
       <c r="I166" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K166" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -23622,8 +24129,11 @@
       <c r="I167" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K167" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -23645,8 +24155,11 @@
       <c r="I168" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K168" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -23668,8 +24181,11 @@
       <c r="I169" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K169" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -23691,8 +24207,11 @@
       <c r="I170" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K170" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -23714,8 +24233,11 @@
       <c r="I171" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K171" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -23737,8 +24259,11 @@
       <c r="I172" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K172" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -23760,8 +24285,11 @@
       <c r="I173" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K173" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -23783,8 +24311,11 @@
       <c r="I174" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K174" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -23806,8 +24337,11 @@
       <c r="I175" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K175" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -23829,8 +24363,11 @@
       <c r="I176" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K176" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -23852,8 +24389,11 @@
       <c r="I177" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K177" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -23875,8 +24415,11 @@
       <c r="I178" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K178" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -23898,8 +24441,11 @@
       <c r="I179" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K179" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -23921,8 +24467,11 @@
       <c r="I180" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K180" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -23944,8 +24493,11 @@
       <c r="I181" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K181" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -23967,8 +24519,11 @@
       <c r="I182" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K182" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -23990,8 +24545,11 @@
       <c r="I183" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K183" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -24013,8 +24571,11 @@
       <c r="I184" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K184" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A185" s="23">
         <v>184</v>
       </c>
@@ -24041,8 +24602,11 @@
         <v>5</v>
       </c>
       <c r="J185" s="23"/>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K185" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A186" s="23">
         <v>185</v>
       </c>
@@ -24069,8 +24633,11 @@
         <v>5</v>
       </c>
       <c r="J186" s="23"/>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K186" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A187" s="23">
         <v>186</v>
       </c>
@@ -24097,8 +24664,11 @@
         <v>5</v>
       </c>
       <c r="J187" s="23"/>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K187" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A188" s="23">
         <v>187</v>
       </c>
@@ -24125,8 +24695,11 @@
         <v>5</v>
       </c>
       <c r="J188" s="23"/>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K188" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A189" s="23">
         <v>188</v>
       </c>
@@ -24153,8 +24726,11 @@
         <v>5</v>
       </c>
       <c r="J189" s="23"/>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K189" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A190" s="23">
         <v>189</v>
       </c>
@@ -24181,8 +24757,11 @@
         <v>5</v>
       </c>
       <c r="J190" s="23"/>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K190" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A191" s="23">
         <v>190</v>
       </c>
@@ -24209,8 +24788,11 @@
         <v>5</v>
       </c>
       <c r="J191" s="23"/>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K191" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A192" s="23">
         <v>191</v>
       </c>
@@ -24237,8 +24819,11 @@
         <v>5</v>
       </c>
       <c r="J192" s="23"/>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K192" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A193" s="23">
         <v>192</v>
       </c>
@@ -24265,8 +24850,11 @@
         <v>5</v>
       </c>
       <c r="J193" s="23"/>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K193" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A194" s="23">
         <v>193</v>
       </c>
@@ -24293,8 +24881,11 @@
         <v>5</v>
       </c>
       <c r="J194" s="23"/>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K194" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A195" s="23">
         <v>194</v>
       </c>
@@ -24321,8 +24912,11 @@
         <v>5</v>
       </c>
       <c r="J195" s="23"/>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K195" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A196" s="23">
         <v>195</v>
       </c>
@@ -24349,8 +24943,11 @@
         <v>5</v>
       </c>
       <c r="J196" s="23"/>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K196" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A197" s="23">
         <v>196</v>
       </c>
@@ -24377,8 +24974,11 @@
         <v>5</v>
       </c>
       <c r="J197" s="23"/>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K197" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A198" s="23">
         <v>197</v>
       </c>
@@ -24405,8 +25005,11 @@
         <v>5</v>
       </c>
       <c r="J198" s="23"/>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K198" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A199" s="23">
         <v>198</v>
       </c>
@@ -24433,8 +25036,11 @@
         <v>5</v>
       </c>
       <c r="J199" s="23"/>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K199" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A200" s="23">
         <v>199</v>
       </c>
@@ -24461,8 +25067,11 @@
         <v>5</v>
       </c>
       <c r="J200" s="23"/>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K200" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A201" s="23">
         <v>200</v>
       </c>
@@ -24489,8 +25098,11 @@
         <v>5</v>
       </c>
       <c r="J201" s="23"/>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K201" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A202" s="23">
         <v>201</v>
       </c>
@@ -24517,8 +25129,11 @@
         <v>5</v>
       </c>
       <c r="J202" s="23"/>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K202" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A203" s="23">
         <v>202</v>
       </c>
@@ -24545,8 +25160,11 @@
         <v>5</v>
       </c>
       <c r="J203" s="23"/>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K203" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A204" s="23">
         <v>203</v>
       </c>
@@ -24573,8 +25191,11 @@
         <v>5</v>
       </c>
       <c r="J204" s="23"/>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K204" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A205" s="23">
         <v>204</v>
       </c>
@@ -24601,8 +25222,11 @@
         <v>5</v>
       </c>
       <c r="J205" s="23"/>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K205" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A206" s="23">
         <v>205</v>
       </c>
@@ -24629,8 +25253,11 @@
         <v>5</v>
       </c>
       <c r="J206" s="23"/>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K206" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A207" s="23">
         <v>206</v>
       </c>
@@ -24657,8 +25284,11 @@
         <v>5</v>
       </c>
       <c r="J207" s="23"/>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K207" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A208" s="23">
         <v>207</v>
       </c>
@@ -24685,8 +25315,11 @@
         <v>5</v>
       </c>
       <c r="J208" s="23"/>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K208" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A209" s="23">
         <v>208</v>
       </c>
@@ -24713,8 +25346,11 @@
         <v>6</v>
       </c>
       <c r="J209" s="23"/>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K209" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A210" s="23">
         <v>209</v>
       </c>
@@ -24741,8 +25377,11 @@
         <v>6</v>
       </c>
       <c r="J210" s="23"/>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K210" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A211" s="23">
         <v>210</v>
       </c>
@@ -24769,8 +25408,11 @@
         <v>6</v>
       </c>
       <c r="J211" s="23"/>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K211" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A212" s="23">
         <v>211</v>
       </c>
@@ -24797,8 +25439,11 @@
         <v>6</v>
       </c>
       <c r="J212" s="23"/>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K212" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A213" s="23">
         <v>212</v>
       </c>
@@ -24825,8 +25470,11 @@
         <v>6</v>
       </c>
       <c r="J213" s="23"/>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K213" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A214" s="23">
         <v>213</v>
       </c>
@@ -24853,8 +25501,11 @@
         <v>6</v>
       </c>
       <c r="J214" s="23"/>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K214" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A215" s="23">
         <v>214</v>
       </c>
@@ -24881,8 +25532,11 @@
         <v>6</v>
       </c>
       <c r="J215" s="23"/>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K215" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A216" s="23">
         <v>215</v>
       </c>
@@ -24909,8 +25563,11 @@
         <v>6</v>
       </c>
       <c r="J216" s="23"/>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K216" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A217" s="23">
         <v>216</v>
       </c>
@@ -24937,8 +25594,11 @@
         <v>6</v>
       </c>
       <c r="J217" s="23"/>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K217" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A218" s="23">
         <v>217</v>
       </c>
@@ -24965,8 +25625,11 @@
         <v>6</v>
       </c>
       <c r="J218" s="23"/>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K218" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A219" s="23">
         <v>218</v>
       </c>
@@ -24993,8 +25656,11 @@
         <v>6</v>
       </c>
       <c r="J219" s="23"/>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K219" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A220" s="23">
         <v>219</v>
       </c>
@@ -25021,8 +25687,11 @@
         <v>6</v>
       </c>
       <c r="J220" s="23"/>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K220" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A221" s="23">
         <v>220</v>
       </c>
@@ -25049,8 +25718,11 @@
         <v>6</v>
       </c>
       <c r="J221" s="23"/>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K221" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A222" s="23">
         <v>221</v>
       </c>
@@ -25077,8 +25749,11 @@
         <v>6</v>
       </c>
       <c r="J222" s="23"/>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K222" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A223" s="23">
         <v>222</v>
       </c>
@@ -25105,8 +25780,11 @@
         <v>6</v>
       </c>
       <c r="J223" s="23"/>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K223" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A224" s="23">
         <v>223</v>
       </c>
@@ -25133,8 +25811,11 @@
         <v>6</v>
       </c>
       <c r="J224" s="23"/>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K224" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A225" s="23">
         <v>224</v>
       </c>
@@ -25161,8 +25842,11 @@
         <v>6</v>
       </c>
       <c r="J225" s="23"/>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K225" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A226" s="23">
         <v>225</v>
       </c>
@@ -25189,8 +25873,11 @@
         <v>6</v>
       </c>
       <c r="J226" s="23"/>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K226" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A227" s="23">
         <v>226</v>
       </c>
@@ -25217,8 +25904,11 @@
         <v>6</v>
       </c>
       <c r="J227" s="23"/>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K227" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A228" s="23">
         <v>227</v>
       </c>
@@ -25245,8 +25935,11 @@
         <v>6</v>
       </c>
       <c r="J228" s="23"/>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K228" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A229" s="23">
         <v>228</v>
       </c>
@@ -25273,8 +25966,11 @@
         <v>6</v>
       </c>
       <c r="J229" s="23"/>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K229" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A230" s="23">
         <v>229</v>
       </c>
@@ -25301,8 +25997,11 @@
         <v>6</v>
       </c>
       <c r="J230" s="23"/>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K230" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A231" s="23">
         <v>230</v>
       </c>
@@ -25329,8 +26028,11 @@
         <v>6</v>
       </c>
       <c r="J231" s="23"/>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K231" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A232" s="23">
         <v>231</v>
       </c>
@@ -25357,8 +26059,11 @@
         <v>6</v>
       </c>
       <c r="J232" s="23"/>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K232" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A233" s="23">
         <v>232</v>
       </c>
@@ -25385,8 +26090,11 @@
         <v>6</v>
       </c>
       <c r="J233" s="23"/>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K233" s="1" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A234" s="23">
         <v>233</v>
       </c>
@@ -25413,6 +26121,9 @@
         <v>6</v>
       </c>
       <c r="J234" s="23"/>
+      <c r="K234" s="1" t="s">
+        <v>2532</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -72204,8 +72915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>